<commit_message>
running on three versions. Config works. Fix clean graphs.
</commit_message>
<xml_diff>
--- a/CldMaker/dataset/prompts_vars.xlsx
+++ b/CldMaker/dataset/prompts_vars.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10811"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10910"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Georgia 1/CldMaker-1/CldMaker/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Georgia 1/CldMaker-1/CldMaker/dataset/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{FAD7D202-48DB-7742-AD1C-A279AB9F8C6C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{748B62A8-529E-DD47-87FE-B35B61AA88A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5180" yWindow="1800" windowWidth="28040" windowHeight="17440"/>
+    <workbookView xWindow="1140" yWindow="1620" windowWidth="32680" windowHeight="19000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="prompts_vars" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="65">
   <si>
     <t>Case</t>
   </si>
@@ -32,9 +32,6 @@
   </si>
   <si>
     <t>label_graphs</t>
-  </si>
-  <si>
-    <t>Unnamed: 4</t>
   </si>
   <si>
     <t>nx_graph</t>
@@ -223,9 +220,6 @@
 "market price" -&gt; "retail car sales"[arrowhead = tee]
 "retail car sales"-&gt; "inventory of cars at dealership"[arrowhead = tee]
 }</t>
-  </si>
-  <si>
-    <t>p102</t>
   </si>
   <si>
     <t>DiGraph with 4 nodes and 5 edges</t>
@@ -245,9 +239,6 @@
 "brith rate"-&gt;"births"[arrowhead = vee] 
 "death rate"-&gt;"deaths"[arrowhead = vee] 
 }</t>
-  </si>
-  <si>
-    <t>p99</t>
   </si>
   <si>
     <t>DiGraph with 5 nodes and 6 edges</t>
@@ -274,16 +265,82 @@
 }</t>
   </si>
   <si>
-    <t>p108</t>
-  </si>
-  <si>
     <t>DiGraph with 8 nodes and 11 edges</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> The Assignment Backlog is increased by the Assignment Rate and decreased by the Completion Rate. Completion Rate (taskdweek) is Workweek (hours per week) times Productivity (tasks completed per hour of effort) times the Effort Devoted to Assignments. Effort Devoted to Assignments is the effort put in by the student compared to the effort required to complete the assignment with high quality. If work pressure is high, the student may choose to cut corners, skim some reading, skip classes, or give less complete answers to the questions in assignments. For example, if a student works 50 hours per week and can do one task per hour with high quality but only does half the work each assignment requires for a good job, then the completion rate would be (50)(1)(.5) = 25 task equivalents per week.
+Work Pressure determines the workweek and effort devoted to assignments. Work pressure depends on the assignment backlog and the Time Remaining to complete the work: The bigger the backlog or the less time remaining, the higher the workweek needs to be to complete the work on time. Time remaining is of course simply the difference between the Due Date and the current Calendar Time. The two most basic options available to a student faced with high work pressure are to (1) work longer hours, thus increasing the completion rate and reducing the backlog (the Midnight Oil loop B l), or (2) work faster by spending less time on each task, speeding the completion rate and reducing the backlog (the Corner Cutting loop B2). Both are negative feedbacks whose goal is to reduce work pressure to a tolerable level.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Reference </t>
+  </si>
+  <si>
+    <t>digraph{
+    "Assignment Backlog" -&gt; "Work Pressure" [arrowhead= vee]
+    "Work Pressure" -&gt; "Workweek" [arrowhead= vee] 
+    "Workweek" -&gt; "Work Completion Rate"  [arrowhead= tee] 
+    "Work Completion Rate" -&gt; "Assignment Backlog" [arrowhead= tee]
+    "Work Pressure" -&gt; "Effort Devoted to Assignments" [arrowhead= tee]
+    "Effort Devoted to Assignments" -&gt; "Work Completion Rate" [arrowhead= tee]
+    "Assignment Rate" -&gt; "Assignment Backlog" [arrowhead= vee]
+    "Time Remaining" -&gt; "Work Pressure" [arrowhead= tee] 
+    "Due Date" -&gt; "Time Remaining" [arrowhead= vee] 
+    "Calendar Time" -&gt; "Time Remaining" [arrowhead= tee] 
+    "Productivity" -&gt; "Work Completion Rate"  [arrowhead= vee] 
+}</t>
+  </si>
+  <si>
+    <t>A high-tech organization grows rapidly because of its ability to introduce new products. As new products grow, revenues grow, the R&amp;D budget grows, and the engineering and research staff grows. Eventually, this burgeoning technical staff becomes increasingly complex and difficult to manage. The management burden often falls on senior engineers, who in turn have less time to spend on engineering. Diverting the most experienced engineers from engineering to management results in longer product development  times, which slow down the introduction of new products.</t>
+  </si>
+  <si>
+    <t>In most firms the advertising budget (supporting ads, trade shows, and the like) grows roughly as the company and revenue grow. Larger advertising budgets have two effects: (1) more potential customers are made aware of the product and choose to enter the market; (2) to the extent the advertising is effective, more of those who are aware and in the market are likely to buy the product offered by the company . Similarly, the larger the revenue of the firm, the greater the sales budget. The more sales representatives, and the greater their skill and experience, the more calls they can make, the more time they can spend with customers, and the more effective their calls will be, increasing both total industry demand. and the share of the total demand won by the firm.</t>
+  </si>
+  <si>
+    <t>digraph{
+    "Sales" -&gt; "Revenue" [arrowhead= vee]
+    "Revenue" -&gt; "Advertising" [arrowhead= vee] 
+    "Advertising" -&gt; "Market Share"  [arrowhead= vee] 
+    "Market Share" -&gt; "Sales" [arrowhead= vee]
+    "Advertising" -&gt; "Industry Demand" [arrowhead= vee]
+    "Industry Demand" -&gt; "Sales" [arrowhead= vee]
+    "Direct Sales Capabilities" -&gt; "Market Share" [arrowhead= vee]
+    "Revenue" -&gt; "Direct Sales Capabilities" [arrowhead= vee]
+    "Direct Sales Capabilities" -&gt; "Industry Demand" [arrowhead= vee] 
+    "Product Attractiveness" -&gt; "Industry Demand" [arrowhead= vee] 
+       "Product Attractiveness" -&gt; "Market Share" [arrowhead= vee] 
+}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Morale grows and talented junior members are highly motivated, expecting to become partners within ten years. But as the firm gets larger, its growth slows. Perhaps it starts to saturate its market niche. Or it might reach a size where the founding partners are no longer interested in sustaining rapid growth. However the growth rate slows, this means less promotion opportunities, more in-fighting among junior members, and an overall decline in morale. The limits to growth structure can be diagrammed as follows. </t>
+  </si>
+  <si>
+    <t>digraph{
+  "Motivation and Productivity" -&gt; "Growth" [arrowhead = vee]
+   "Growth" -&gt; "Promotion Opportunites" [arrowhead = vee]
+   "Promotion Opportunites" -&gt; "Morale" [arrowhead = vee]
+   "Morale" -&gt; "Motivation and Productivity" [arrowhead = vee]
+    "Growth" -&gt; "Staturation of Market Niche"[arrowhead = tee]
+     "Staturation of Market Niche" -&gt; "Growth" [arrowhead = vee]
+    "Size of Market Niche" -&gt; "Staturation of Market Niche" [arrowhead = tee]
+}</t>
+  </si>
+  <si>
+    <t>digraph{
+   "RD budget"-&gt; "Size of Engineering Staff" [arrowhead = vee]
+   "Size of Engineering Staff" -&gt; "Management Complexity" [arrowhead = vee]
+   "Management Complexity" -&gt; "Management Burden to senior engineers" [arrowhead = vee]
+   "Management Burden to senior engineers" -&gt; "Product Development time" [arrowhead = vee]
+    "Product Development time" -&gt; "New Products"[arrowhead = tee]
+     "New Products" -&gt; "Revenues" [arrowhead = vee]
+    "Revenues" -&gt; "RD budget" [arrowhead = vee]
+    "RD budget" -&gt;  "New Products" [arrowhead = vee]
+}</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -761,10 +818,13 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="42">
@@ -1120,298 +1180,345 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F16"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:F20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="C20" sqref="C20"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="6.5" style="1" customWidth="1"/>
+    <col min="2" max="2" width="60.83203125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="37.33203125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="70" style="1" customWidth="1"/>
+    <col min="5" max="5" width="26.83203125" style="1" customWidth="1"/>
+    <col min="6" max="7" width="15.33203125" style="1" customWidth="1"/>
+    <col min="8" max="16384" width="10.83203125" style="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
+    <row r="1" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="102" x14ac:dyDescent="0.2">
+      <c r="A2" s="1">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="B2" t="s">
+      <c r="C2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="E2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="F2" t="s">
+    </row>
+    <row r="3" spans="1:6" ht="102" x14ac:dyDescent="0.2">
+      <c r="A3" s="1">
+        <v>2</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A3">
-        <v>2</v>
-      </c>
-      <c r="B3" t="s">
+      <c r="C3" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="E3" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="136" x14ac:dyDescent="0.2">
+      <c r="A4" s="1">
+        <v>3</v>
+      </c>
+      <c r="B4" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="F3" t="s">
+      <c r="C4" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="153" x14ac:dyDescent="0.2">
+      <c r="A5" s="1">
+        <v>4</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="85" x14ac:dyDescent="0.2">
+      <c r="A6" s="1">
+        <v>5</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="119" x14ac:dyDescent="0.2">
+      <c r="A7" s="1">
+        <v>6</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="85" x14ac:dyDescent="0.2">
+      <c r="A8" s="1">
+        <v>7</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="170" x14ac:dyDescent="0.2">
+      <c r="A9" s="1">
+        <v>8</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="102" x14ac:dyDescent="0.2">
+      <c r="A10" s="1">
         <v>9</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A4">
-        <v>3</v>
-      </c>
-      <c r="B4" t="s">
+      <c r="B10" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="136" x14ac:dyDescent="0.2">
+      <c r="A11" s="1">
+        <v>10</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="85" x14ac:dyDescent="0.2">
+      <c r="A12" s="1">
+        <v>11</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="102" x14ac:dyDescent="0.2">
+      <c r="A13" s="1">
+        <v>12</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="238" x14ac:dyDescent="0.2">
+      <c r="A14" s="1">
         <v>13</v>
       </c>
-      <c r="C4" t="s">
+      <c r="B14" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" ht="136" x14ac:dyDescent="0.2">
+      <c r="A15" s="1">
         <v>14</v>
       </c>
-      <c r="D4" s="1" t="s">
+      <c r="B15" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" ht="221" x14ac:dyDescent="0.2">
+      <c r="A16" s="1">
         <v>15</v>
       </c>
-      <c r="F4" t="s">
+      <c r="B16" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="409.6" x14ac:dyDescent="0.2">
+      <c r="A17" s="1">
         <v>16</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A5">
-        <v>4</v>
-      </c>
-      <c r="B5" t="s">
+      <c r="B17" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="221" x14ac:dyDescent="0.2">
+      <c r="A18" s="1">
         <v>17</v>
       </c>
-      <c r="C5" t="s">
+      <c r="B18" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="204" x14ac:dyDescent="0.2">
+      <c r="A19" s="1">
         <v>18</v>
       </c>
-      <c r="D5" s="1" t="s">
+      <c r="B19" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" ht="153" x14ac:dyDescent="0.2">
+      <c r="A20" s="1">
         <v>19</v>
       </c>
-      <c r="F5" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A6">
-        <v>5</v>
-      </c>
-      <c r="B6" t="s">
-        <v>20</v>
-      </c>
-      <c r="C6" t="s">
-        <v>21</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="F6" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A7">
-        <v>6</v>
-      </c>
-      <c r="B7" t="s">
-        <v>23</v>
-      </c>
-      <c r="C7" t="s">
-        <v>24</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="F7" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A8">
-        <v>7</v>
-      </c>
-      <c r="B8" t="s">
-        <v>27</v>
-      </c>
-      <c r="C8" t="s">
-        <v>28</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="F8" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A9">
-        <v>8</v>
-      </c>
-      <c r="B9" t="s">
-        <v>30</v>
-      </c>
-      <c r="C9" t="s">
-        <v>31</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="F9" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A10">
-        <v>9</v>
-      </c>
-      <c r="B10" t="s">
-        <v>33</v>
-      </c>
-      <c r="C10" t="s">
-        <v>34</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="F10" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A11">
-        <v>10</v>
-      </c>
-      <c r="B11" t="s">
-        <v>36</v>
-      </c>
-      <c r="C11" t="s">
-        <v>37</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="F11" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A12">
-        <v>11</v>
-      </c>
-      <c r="B12" t="s">
-        <v>39</v>
-      </c>
-      <c r="C12" t="s">
-        <v>40</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="F12" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A13">
-        <v>12</v>
-      </c>
-      <c r="B13" t="s">
-        <v>42</v>
-      </c>
-      <c r="C13" t="s">
-        <v>43</v>
-      </c>
-      <c r="D13" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="F13" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A14">
-        <v>13</v>
-      </c>
-      <c r="B14" t="s">
-        <v>45</v>
-      </c>
-      <c r="C14" t="s">
-        <v>46</v>
-      </c>
-      <c r="D14" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="E14" t="s">
-        <v>48</v>
-      </c>
-      <c r="F14" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A15">
-        <v>14</v>
-      </c>
-      <c r="B15" t="s">
-        <v>50</v>
-      </c>
-      <c r="C15" t="s">
-        <v>51</v>
-      </c>
-      <c r="D15" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="E15" t="s">
-        <v>53</v>
-      </c>
-      <c r="F15" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A16">
-        <v>15</v>
-      </c>
-      <c r="B16" t="s">
-        <v>55</v>
-      </c>
-      <c r="C16" t="s">
-        <v>56</v>
-      </c>
-      <c r="D16" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="E16" t="s">
-        <v>58</v>
-      </c>
-      <c r="F16" t="s">
-        <v>59</v>
+      <c r="B20" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>63</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>